<commit_message>
S_PM_07 task added successfully
</commit_message>
<xml_diff>
--- a/Project Management Crash Course-BC/S_PM_07.xlsx
+++ b/Project Management Crash Course-BC/S_PM_07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Sprints\Sprints\Project Management Crash Course-BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B31C287-81CF-48A7-A9CC-58B6652543DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6739D2-B797-4C77-B156-3AAAF4745941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C8CD34B-ACFB-4B44-AE27-105845B1F712}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
     <t>Yes, the project is over budget by 1500 hrs.</t>
   </si>
   <si>
-    <t>No, it is ahead by 500 hrs, which is equivalent to 10 days (5 Engineers, 9 Working Hrs/Day)</t>
+    <t>No, it is ahead by 500 hrs, which is equivalent to 12.5 days (5 Engineers, 10 Working Hrs/Day)</t>
   </si>
 </sst>
 </file>
@@ -341,32 +340,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -656,25 +629,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -772,25 +726,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -910,542 +845,6 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="34925" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1785,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4927BC83-B266-4B6D-8E0A-14A2824F638E}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1794,8 +1193,9 @@
     <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.88671875" style="1"/>
     <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="74.21875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="7.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="86.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
S_PM_07 task modified successfully
</commit_message>
<xml_diff>
--- a/Project Management Crash Course-BC/S_PM_07.xlsx
+++ b/Project Management Crash Course-BC/S_PM_07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Sprints\Sprints\Project Management Crash Course-BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6739D2-B797-4C77-B156-3AAAF4745941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5E6F64-CA39-40E5-BAB2-D4FCCD23558A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C8CD34B-ACFB-4B44-AE27-105845B1F712}"/>
   </bookViews>
@@ -484,10 +484,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$C$2:$C$4</c:f>
+              <c:f>'Sheet 1'!$C$2:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -556,10 +556,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$D$2:$D$4</c:f>
+              <c:f>'Sheet 1'!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1184,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4927BC83-B266-4B6D-8E0A-14A2824F638E}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>